<commit_message>
change hop dong template
</commit_message>
<xml_diff>
--- a/src/template/EmployeeList.xlsx
+++ b/src/template/EmployeeList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taoda\tools\xls2doc\src\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taoda\tools\xls2docs\src\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F54CF2-7405-4968-9630-7F16BEC0A99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820E5317-1AE4-44FC-B58E-8BE938024F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11040" xr2:uid="{98AD94BF-A7CA-4881-94D3-E4FC97A617FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11310" xr2:uid="{98AD94BF-A7CA-4881-94D3-E4FC97A617FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,9 +451,6 @@
     <t>SalaryText</t>
   </si>
   <si>
-    <t>Tây Vinh, Tây Sơn, Bình Định</t>
-  </si>
-  <si>
     <t>Kinh tế</t>
   </si>
   <si>
@@ -493,9 +490,6 @@
     <t>Nguyễn Lâm Sinh</t>
   </si>
   <si>
-    <t>Nhơn Thọ, An Nhơn, Bình Định</t>
-  </si>
-  <si>
     <t>Cử nhân</t>
   </si>
   <si>
@@ -523,9 +517,6 @@
     <t>Phát triển phần mềm PACS; Hỗ trợ xây dựng giải pháp &amp; kiến trúc cho các sản phẩm của công ty</t>
   </si>
   <si>
-    <t>Từ thứ 2 đến thứ  6 (trừ ngày nghỉ lễ theo quy định). Tối đa 8 giờ mỗi ngày và tối đa 40 giờ mỗi tuần</t>
-  </si>
-  <si>
     <t>Tối đa 8 giờ mỗi ngày và tối đa 40 giờ mỗi tuần</t>
   </si>
   <si>
@@ -634,30 +625,6 @@
     <t>Lê Quốc Mạnh</t>
   </si>
   <si>
-    <t>thị trấn KBang, huyện KBang, tỉnh Gia Lai</t>
-  </si>
-  <si>
-    <t>Trung Tín 1, Thị Trấn Tuy Phước, Tuy Phước, Bình Định</t>
-  </si>
-  <si>
-    <t>Tổ 3 phường Phù Đổng, thành phố Pleiku, Gia Lai</t>
-  </si>
-  <si>
-    <t>Phường Ngô Mây, thành phố Quy Nhơn,tỉnh Bình Định</t>
-  </si>
-  <si>
-    <t>Cát Chánh, Phù cát, Bình Định</t>
-  </si>
-  <si>
-    <t>44/76/2 Trần Hưng Đạo, P.Hải Cảng, Quy Nhơn, Bình Định</t>
-  </si>
-  <si>
-    <t>Mỹ Thọ, Phù Mỹ, Bình Định</t>
-  </si>
-  <si>
-    <t>Cát Thành, Phù Cát, Bình Định</t>
-  </si>
-  <si>
     <t>theo tháng</t>
   </si>
   <si>
@@ -746,6 +713,39 @@
   </si>
   <si>
     <t>Thôn Hiển Đông, Canh Hiển, Vân Canh, Bình Định</t>
+  </si>
+  <si>
+    <t>tối đa 8 giờ mỗi ngày và tối đa 40 giờ mỗi tuần</t>
+  </si>
+  <si>
+    <t>Thôn Thọ Lộc 1, Nhơn Thọ, An Nhơn, Bình Định</t>
+  </si>
+  <si>
+    <t>Thôn An Vinh 2, Tây Vinh, Tây Sơn, Bình Định</t>
+  </si>
+  <si>
+    <t>Thị trấn KBang, huyện KBang, tỉnh Gia Lai</t>
+  </si>
+  <si>
+    <t>Thôn Phú Trung, Cát Thành, Phù Cát, Bình Định</t>
+  </si>
+  <si>
+    <t>Thôn Chánh Đạo, Mỹ Thọ, Phù Mỹ, Bình Định</t>
+  </si>
+  <si>
+    <t>44/76/2 Trần Hưng Đạo, phường Hải Cảng, thành phố Quy Nhơn, tỉnh Bình Định</t>
+  </si>
+  <si>
+    <t>Thôn Trung Tín 1, Thị Trấn Tuy Phước, Tuy Phước, Bình Định</t>
+  </si>
+  <si>
+    <t>Tổ 3 phường Phù Đổng, thành phố Pleiku, tỉnh Gia Lai</t>
+  </si>
+  <si>
+    <t>Tổ 11, khu vực 2, phường Nhơn Bình, thành phố Quy Nhơn, tỉnh Bình Định</t>
+  </si>
+  <si>
+    <t>Tổ 6, Khu vực 8, phường Ngô Mây, thành phố Quy Nhơn,tỉnh Bình Định</t>
   </si>
 </sst>
 </file>
@@ -760,7 +760,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -781,7 +781,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -794,7 +794,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -1201,38 +1201,38 @@
   <dimension ref="A1:U427"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.125" style="1"/>
+    <col min="3" max="3" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="1"/>
+    <col min="5" max="5" width="15.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" style="1" customWidth="1"/>
-    <col min="18" max="19" width="12.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="20.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.25" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.875" style="1" customWidth="1"/>
+    <col min="18" max="19" width="12.375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.75" style="1" customWidth="1"/>
+    <col min="21" max="21" width="23.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -1250,7 +1250,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>5</v>
@@ -1274,19 +1274,19 @@
         <v>11</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="T1" s="11" t="s">
         <v>12</v>
@@ -1301,62 +1301,62 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3">
         <v>45323</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="3">
         <v>32908</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="I2" s="3">
         <v>44419</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="L2" s="3">
         <v>45323</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="4" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="S2" s="10">
         <v>15000000</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1365,62 +1365,62 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C3" s="3">
         <v>45293</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="3">
         <v>33878</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="I3" s="3">
         <v>44301</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L3" s="3">
         <v>45293</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="S3" s="10">
         <v>14000000</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1429,94 +1429,94 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C4" s="3">
         <v>45323</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3">
         <v>35680</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="I4" s="3">
         <v>44296</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L4" s="3">
         <v>45323</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="4" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="S4" s="10">
         <v>12000000</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f>IF(K5="","",IF(K5="Cộng tác viên",COUNTIF($K$2:K5,"Cộng tác viên"),COUNTA($K$2:K5)-COUNTIF($K$2:K5,"Cộng tác viên")))</f>
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C5" s="3">
         <v>45323</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3">
         <v>33088</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="I5" s="3">
         <v>44401</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L5" s="3">
         <v>45323</v>
@@ -1525,28 +1525,28 @@
         <v>45688</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="O5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="Q5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="S5" s="10">
         <v>30000000</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1555,32 +1555,32 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3">
         <v>45323</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F6" s="3">
         <v>34597</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="I6" s="3">
         <v>44419</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L6" s="3">
         <v>45323</v>
@@ -1589,28 +1589,28 @@
         <v>45688</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="S6" s="10">
         <v>7000000</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1619,32 +1619,32 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C7" s="3">
         <v>45323</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3">
         <v>36067</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="I7" s="3">
         <v>44840</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L7" s="3">
         <v>45323</v>
@@ -1653,28 +1653,28 @@
         <v>45688</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="S7" s="10">
         <v>10000000</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1683,32 +1683,32 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C8" s="3">
         <v>45323</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F8" s="3">
         <v>37533</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="I8" s="3">
         <v>44326</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L8" s="3">
         <v>45323</v>
@@ -1717,28 +1717,28 @@
         <v>45688</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="S8" s="10">
         <v>6500000</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1747,32 +1747,32 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C9" s="3">
         <v>45323</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F9" s="3">
         <v>36193</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="I9" s="3">
         <v>45223</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L9" s="3">
         <v>45323</v>
@@ -1781,28 +1781,28 @@
         <v>45688</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="S9" s="10">
         <v>5500000</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1811,32 +1811,32 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C10" s="3">
         <v>45323</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F10" s="3">
         <v>37052</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="I10" s="3">
         <v>44440</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L10" s="3">
         <v>45323</v>
@@ -1845,28 +1845,28 @@
         <v>45688</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="S10" s="10">
         <v>6000000</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1875,32 +1875,32 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C11" s="3">
         <v>45323</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F11" s="3">
         <v>44525</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="I11" s="3">
         <v>44375</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L11" s="3">
         <v>45323</v>
@@ -1909,28 +1909,28 @@
         <v>45688</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="S11" s="10">
         <v>6000000</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1939,32 +1939,32 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C12" s="3">
         <v>45323</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F12" s="3">
         <v>37174</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="I12" s="3">
         <v>44325</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L12" s="3">
         <v>45323</v>
@@ -1973,28 +1973,28 @@
         <v>45688</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="S12" s="10">
         <v>6000000</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -2003,16 +2003,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C13" s="3">
         <v>45323</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
@@ -2020,7 +2020,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L13" s="3">
         <v>45323</v>
@@ -2029,28 +2029,28 @@
         <v>45688</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="S13" s="10">
         <v>250000</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -3374,21 +3374,21 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gen lai hop dong
</commit_message>
<xml_diff>
--- a/src/template/EmployeeList.xlsx
+++ b/src/template/EmployeeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taoda\tools\xls2docs\src\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820E5317-1AE4-44FC-B58E-8BE938024F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119C81E3-5749-499E-9457-30B76CB7D68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11310" xr2:uid="{98AD94BF-A7CA-4881-94D3-E4FC97A617FC}"/>
   </bookViews>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="114">
   <si>
     <t>No</t>
   </si>
@@ -430,9 +430,6 @@
     <t>IssueDate</t>
   </si>
   <si>
-    <t>Certificate</t>
-  </si>
-  <si>
     <t>ContractType</t>
   </si>
   <si>
@@ -451,9 +448,6 @@
     <t>SalaryText</t>
   </si>
   <si>
-    <t>Kinh tế</t>
-  </si>
-  <si>
     <t>Mười bốn triệu đồng chẵn</t>
   </si>
   <si>
@@ -490,9 +484,6 @@
     <t>Nguyễn Lâm Sinh</t>
   </si>
   <si>
-    <t>Cử nhân</t>
-  </si>
-  <si>
     <t>Nguyễn Trường Hải</t>
   </si>
   <si>
@@ -746,6 +737,18 @@
   </si>
   <si>
     <t>Tổ 6, Khu vực 8, phường Ngô Mây, thành phố Quy Nhơn,tỉnh Bình Định</t>
+  </si>
+  <si>
+    <t>Tổ 9, ấp 3, Phú Điền, Tân Phú, Đồng Nai</t>
+  </si>
+  <si>
+    <t>By</t>
+  </si>
+  <si>
+    <t>Cục CSQLHC về TTXH</t>
+  </si>
+  <si>
+    <t>CA tỉnh Đồng Nai</t>
   </si>
 </sst>
 </file>
@@ -1201,10 +1204,10 @@
   <dimension ref="A1:U427"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1220,7 @@
     <col min="7" max="7" width="26.375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.375" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="9.125" style="1" customWidth="1"/>
     <col min="11" max="11" width="20.75" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="10.375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30.25" style="1" customWidth="1"/>
@@ -1230,9 +1233,9 @@
     <col min="22" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -1250,7 +1253,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>5</v>
@@ -1259,40 +1262,40 @@
         <v>6</v>
       </c>
       <c r="J1" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="T1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="U1" s="11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1301,62 +1304,62 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3">
         <v>45323</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3">
         <v>32908</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I2" s="3">
         <v>44419</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L2" s="3">
         <v>45323</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S2" s="10">
         <v>15000000</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1365,62 +1368,62 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C3" s="3">
         <v>45293</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3">
         <v>33878</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I3" s="3">
         <v>44301</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L3" s="3">
         <v>45293</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S3" s="10">
         <v>14000000</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1429,60 +1432,62 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4" s="3">
         <v>45323</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3">
         <v>35680</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I4" s="3">
         <v>44296</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K4" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L4" s="3">
         <v>45323</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S4" s="10">
         <v>12000000</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -1491,32 +1496,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C5" s="3">
         <v>45323</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5" s="3">
         <v>33088</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I5" s="3">
         <v>44401</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="J5" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K5" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L5" s="3">
         <v>45323</v>
@@ -1525,28 +1532,28 @@
         <v>45688</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S5" s="10">
         <v>30000000</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1555,32 +1562,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C6" s="3">
         <v>45323</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" s="3">
         <v>34597</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I6" s="3">
         <v>44419</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K6" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L6" s="3">
         <v>45323</v>
@@ -1589,28 +1598,28 @@
         <v>45688</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S6" s="10">
         <v>7000000</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1619,32 +1628,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C7" s="3">
         <v>45323</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F7" s="3">
         <v>36067</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I7" s="3">
         <v>44840</v>
       </c>
-      <c r="J7" s="4"/>
+      <c r="J7" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K7" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L7" s="3">
         <v>45323</v>
@@ -1653,28 +1664,28 @@
         <v>45688</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S7" s="10">
         <v>10000000</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1683,32 +1694,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C8" s="3">
         <v>45323</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F8" s="3">
         <v>37533</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I8" s="3">
         <v>44326</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K8" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L8" s="3">
         <v>45323</v>
@@ -1717,28 +1730,28 @@
         <v>45688</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S8" s="10">
         <v>6500000</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1747,32 +1760,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C9" s="3">
         <v>45323</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F9" s="3">
         <v>36193</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I9" s="3">
         <v>45223</v>
       </c>
-      <c r="J9" s="4"/>
+      <c r="J9" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K9" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L9" s="3">
         <v>45323</v>
@@ -1781,28 +1796,28 @@
         <v>45688</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S9" s="10">
         <v>5500000</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1811,32 +1826,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C10" s="3">
         <v>45323</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F10" s="3">
         <v>37052</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I10" s="3">
         <v>44440</v>
       </c>
-      <c r="J10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K10" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L10" s="3">
         <v>45323</v>
@@ -1845,28 +1862,28 @@
         <v>45688</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S10" s="10">
         <v>6000000</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1875,32 +1892,34 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C11" s="3">
         <v>45323</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F11" s="3">
         <v>44525</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I11" s="3">
         <v>44375</v>
       </c>
-      <c r="J11" s="4"/>
+      <c r="J11" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K11" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L11" s="3">
         <v>45323</v>
@@ -1909,28 +1928,28 @@
         <v>45688</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S11" s="10">
         <v>6000000</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1939,32 +1958,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C12" s="3">
         <v>45323</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F12" s="3">
         <v>37174</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I12" s="3">
         <v>44325</v>
       </c>
-      <c r="J12" s="4"/>
+      <c r="J12" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K12" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L12" s="3">
         <v>45323</v>
@@ -1973,28 +1994,28 @@
         <v>45688</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S12" s="10">
         <v>6000000</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -2003,24 +2024,34 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C13" s="3">
         <v>45323</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="F13" s="3">
+        <v>35495</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H13" s="4">
+        <v>272524872</v>
+      </c>
+      <c r="I13" s="3">
+        <v>41060</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="K13" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L13" s="3">
         <v>45323</v>
@@ -2029,28 +2060,28 @@
         <v>45688</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S13" s="10">
         <v>250000</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -3382,13 +3413,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>